<commit_message>
Se creo un nuevo FORM desde el cual se terminará de cargar todas las lecturas procesadas - se modifico el FORM que controla la subida y actualización del padró de clientes - se modifico el procesamiento de datos - se modifico el FORM de ayud/Créditos - se agrego un dependencia para la conexión al archivo EXCEl - se Modífico la tabla DB Clientes, ahora carga todo el archivo Excel que contiene el padrón
</commit_message>
<xml_diff>
--- a/Recursos/LECTURAS REMOTAS SEPTIEMBRE 2018.xlsx
+++ b/Recursos/LECTURAS REMOTAS SEPTIEMBRE 2018.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sing_\source\Electro\Recursos\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="240" windowWidth="15570" windowHeight="9000"/>
   </bookViews>
@@ -13,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'1'!$A$2:$AQ$185</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -1817,7 +1822,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="5">
     <numFmt numFmtId="164" formatCode="0.000000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
@@ -2860,6 +2865,9 @@
     <xf numFmtId="166" fontId="0" fillId="11" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2868,9 +2876,6 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -3154,7 +3159,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3165,10 +3170,10 @@
   <dimension ref="A1:AQ194"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="64" zoomScaleNormal="64" workbookViewId="0">
-      <pane xSplit="5" ySplit="2" topLeftCell="X3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="5" ySplit="2" topLeftCell="L104" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="AJ29" sqref="AJ29:AQ29"/>
+      <selection pane="bottomRight" activeCell="I113" sqref="I113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3178,35 +3183,40 @@
     <col min="3" max="3" width="14.42578125" style="13" customWidth="1"/>
     <col min="4" max="4" width="37.42578125" style="31" customWidth="1"/>
     <col min="5" max="5" width="36.85546875" style="13" customWidth="1"/>
-    <col min="6" max="6" width="10" style="13" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="12.42578125" style="113" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="16.85546875" style="13" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5703125" style="13" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="15.42578125" style="13" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="10.5703125" style="13" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="13.85546875" style="13" customWidth="1"/>
-    <col min="13" max="13" width="17.5703125" style="13" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="14.7109375" style="13" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="5.85546875" style="13" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="7.5703125" style="13" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="11.85546875" style="13" hidden="1" customWidth="1"/>
-    <col min="18" max="18" width="8" style="13" customWidth="1"/>
-    <col min="19" max="19" width="6" style="13" customWidth="1"/>
+    <col min="6" max="6" width="28.5703125" style="13" customWidth="1"/>
+    <col min="7" max="7" width="49" style="113" customWidth="1"/>
+    <col min="8" max="8" width="28" style="13" customWidth="1"/>
+    <col min="9" max="9" width="30.7109375" style="13" customWidth="1"/>
+    <col min="10" max="10" width="19.85546875" style="13" customWidth="1"/>
+    <col min="11" max="11" width="23.28515625" style="13" customWidth="1"/>
+    <col min="12" max="12" width="19" style="13" customWidth="1"/>
+    <col min="13" max="13" width="29.5703125" style="13" customWidth="1"/>
+    <col min="14" max="14" width="22.5703125" style="13" customWidth="1"/>
+    <col min="15" max="15" width="27" style="13" customWidth="1"/>
+    <col min="16" max="16" width="18" style="13" customWidth="1"/>
+    <col min="17" max="17" width="21" style="13" customWidth="1"/>
+    <col min="18" max="18" width="25.5703125" style="13" customWidth="1"/>
+    <col min="19" max="19" width="17.5703125" style="13" customWidth="1"/>
     <col min="20" max="20" width="10.42578125" style="31" customWidth="1"/>
-    <col min="21" max="25" width="10.42578125" style="13" customWidth="1"/>
+    <col min="21" max="21" width="100.7109375" style="13" customWidth="1"/>
+    <col min="22" max="22" width="21.140625" style="13" customWidth="1"/>
+    <col min="23" max="23" width="18" style="13" customWidth="1"/>
+    <col min="24" max="24" width="18.85546875" style="13" customWidth="1"/>
+    <col min="25" max="25" width="23.5703125" style="13" customWidth="1"/>
     <col min="26" max="26" width="7.85546875" style="13" customWidth="1"/>
     <col min="27" max="27" width="16.140625" style="13" customWidth="1"/>
-    <col min="28" max="28" width="7.5703125" style="13" hidden="1" customWidth="1"/>
-    <col min="29" max="30" width="5.42578125" style="13" hidden="1" customWidth="1"/>
-    <col min="31" max="31" width="9.5703125" style="13" hidden="1" customWidth="1"/>
-    <col min="32" max="32" width="6.85546875" style="33" hidden="1" customWidth="1"/>
-    <col min="33" max="33" width="6.85546875" style="33" customWidth="1"/>
-    <col min="34" max="34" width="5.5703125" style="108" customWidth="1"/>
-    <col min="35" max="35" width="2.7109375" style="13" hidden="1" customWidth="1"/>
+    <col min="28" max="28" width="13.42578125" style="13" customWidth="1"/>
+    <col min="29" max="29" width="12.28515625" style="13" customWidth="1"/>
+    <col min="30" max="30" width="14.85546875" style="13" customWidth="1"/>
+    <col min="31" max="31" width="20" style="13" customWidth="1"/>
+    <col min="32" max="32" width="13.28515625" style="33" customWidth="1"/>
+    <col min="33" max="33" width="9.7109375" style="33" customWidth="1"/>
+    <col min="34" max="34" width="9.5703125" style="108" customWidth="1"/>
+    <col min="35" max="35" width="9.5703125" style="13" customWidth="1"/>
     <col min="36" max="36" width="10.7109375" style="34" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="9.7109375" style="34" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="8" style="35" customWidth="1"/>
-    <col min="39" max="39" width="13.7109375" style="113" customWidth="1"/>
+    <col min="39" max="39" width="37" style="113" customWidth="1"/>
     <col min="40" max="40" width="7.42578125" style="13" bestFit="1" customWidth="1"/>
     <col min="41" max="41" width="11.42578125" style="34" customWidth="1"/>
     <col min="42" max="42" width="11.42578125" style="35" bestFit="1" customWidth="1"/>
@@ -3218,51 +3228,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:43" ht="18" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="250" t="s">
+      <c r="A1" s="251" t="s">
         <v>550</v>
       </c>
-      <c r="B1" s="251"/>
-      <c r="C1" s="251"/>
-      <c r="D1" s="251"/>
-      <c r="E1" s="251"/>
-      <c r="F1" s="251"/>
-      <c r="G1" s="252"/>
-      <c r="H1" s="251"/>
-      <c r="I1" s="251"/>
-      <c r="J1" s="251"/>
-      <c r="K1" s="251"/>
-      <c r="L1" s="251"/>
-      <c r="M1" s="251"/>
-      <c r="N1" s="251"/>
-      <c r="O1" s="251"/>
-      <c r="P1" s="251"/>
-      <c r="Q1" s="251"/>
-      <c r="R1" s="251"/>
-      <c r="S1" s="251"/>
-      <c r="T1" s="251"/>
-      <c r="U1" s="251"/>
-      <c r="V1" s="251"/>
-      <c r="W1" s="251"/>
-      <c r="X1" s="251"/>
-      <c r="Y1" s="251"/>
-      <c r="Z1" s="251"/>
-      <c r="AA1" s="251"/>
-      <c r="AB1" s="251"/>
-      <c r="AC1" s="251"/>
-      <c r="AD1" s="251"/>
-      <c r="AE1" s="251"/>
-      <c r="AF1" s="251"/>
-      <c r="AG1" s="251"/>
-      <c r="AH1" s="251"/>
-      <c r="AI1" s="251"/>
-      <c r="AJ1" s="251"/>
-      <c r="AK1" s="251"/>
-      <c r="AL1" s="251"/>
-      <c r="AM1" s="252"/>
-      <c r="AN1" s="251"/>
-      <c r="AO1" s="251"/>
-      <c r="AP1" s="251"/>
-      <c r="AQ1" s="251"/>
+      <c r="B1" s="252"/>
+      <c r="C1" s="252"/>
+      <c r="D1" s="252"/>
+      <c r="E1" s="252"/>
+      <c r="F1" s="252"/>
+      <c r="G1" s="253"/>
+      <c r="H1" s="252"/>
+      <c r="I1" s="252"/>
+      <c r="J1" s="252"/>
+      <c r="K1" s="252"/>
+      <c r="L1" s="252"/>
+      <c r="M1" s="252"/>
+      <c r="N1" s="252"/>
+      <c r="O1" s="252"/>
+      <c r="P1" s="252"/>
+      <c r="Q1" s="252"/>
+      <c r="R1" s="252"/>
+      <c r="S1" s="252"/>
+      <c r="T1" s="252"/>
+      <c r="U1" s="252"/>
+      <c r="V1" s="252"/>
+      <c r="W1" s="252"/>
+      <c r="X1" s="252"/>
+      <c r="Y1" s="252"/>
+      <c r="Z1" s="252"/>
+      <c r="AA1" s="252"/>
+      <c r="AB1" s="252"/>
+      <c r="AC1" s="252"/>
+      <c r="AD1" s="252"/>
+      <c r="AE1" s="252"/>
+      <c r="AF1" s="252"/>
+      <c r="AG1" s="252"/>
+      <c r="AH1" s="252"/>
+      <c r="AI1" s="252"/>
+      <c r="AJ1" s="252"/>
+      <c r="AK1" s="252"/>
+      <c r="AL1" s="252"/>
+      <c r="AM1" s="253"/>
+      <c r="AN1" s="252"/>
+      <c r="AO1" s="252"/>
+      <c r="AP1" s="252"/>
+      <c r="AQ1" s="252"/>
     </row>
     <row r="2" spans="1:43" s="28" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="22" t="s">
@@ -24668,7 +24678,7 @@
       <c r="AK182" s="18">
         <v>0.5</v>
       </c>
-      <c r="AL182" s="253">
+      <c r="AL182" s="250">
         <v>0.12889999999999999</v>
       </c>
       <c r="AM182" s="114">

</xml_diff>